<commit_message>
half way through "other labs"
</commit_message>
<xml_diff>
--- a/data/data_from_M/formatted-table/SV 386 and 388 Wallabout Street.xlsx
+++ b/data/data_from_M/formatted-table/SV 386 and 388 Wallabout Street.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="25601"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10509"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mlittle\Documents\Soil Vapor for students\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lindseycovell/Desktop/Spring 2023/Capstone/ehs_capstone_nycdoh/data/data_from_M/formatted-table/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8CE14B47-FE07-41EE-AF13-E0007B00C3F0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{753AE4C1-56E8-6C42-9D1B-B95BF5298687}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2925" yWindow="1455" windowWidth="25410" windowHeight="14145" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="25600" yWindow="2120" windowWidth="16160" windowHeight="21880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Table 1" sheetId="1" r:id="rId1"/>
@@ -735,6 +735,9 @@
     </r>
   </si>
   <si>
+    <t>Chemtech Labs</t>
+  </si>
+  <si>
     <r>
       <rPr>
         <u/>
@@ -750,43 +753,11 @@
         <rFont val="Arial"/>
         <family val="2"/>
       </rPr>
-      <t xml:space="preserve">:
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="6"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">SG2 Suma cannister failed to draw a sample NA   No guidance value or standard available
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="6"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">(a) NYSDOH Guidance for Evaluating Soil Vapor Intrusion in the State of New York, February
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="6"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">(b) USEPA Draft Guidance for Evaluating the Vapor Intrusion to Indoor Air Pathway from Groundwater and Soils
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="6"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>(Subsurface Vapor Intrusion Guidance), Table 2c, Risk=1 x10</t>
+      <t>:
+SG2 Suma cannister failed to draw a sample NA   No guidance value or standard available
+(a) NYSDOH Guidance for Evaluating Soil Vapor Intrusion in the State of New York, February
+(b) USEPA Draft Guidance for Evaluating the Vapor Intrusion to Indoor Air Pathway from Groundwater and Soils
+(Subsurface Vapor Intrusion Guidance), Table 2c, Risk=1 x10</t>
     </r>
     <r>
       <rPr>
@@ -804,29 +775,10 @@
         <rFont val="Arial"/>
         <family val="2"/>
       </rPr>
-      <t xml:space="preserve">* Petroleum Volatile Organic Compounds
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="6"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">** Benzene, toluene, ethylbenzene, xylene
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="6"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>** * Volatile Organic Compounds (excluding acetone)</t>
-    </r>
-  </si>
-  <si>
-    <t>Chemtech Labs</t>
+      <t>* Petroleum Volatile Organic Compounds
+** Benzene, toluene, ethylbenzene, xylene
+** * Volatile Organic Compounds (excluding acetone)</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -968,7 +920,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
@@ -1029,11 +981,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1375,30 +1330,30 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J67"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:B1"/>
+    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="B69" sqref="B69"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="23.33203125" customWidth="1"/>
-    <col min="2" max="2" width="12.33203125" customWidth="1"/>
-    <col min="3" max="3" width="11.1640625" customWidth="1"/>
-    <col min="4" max="4" width="9.33203125" customWidth="1"/>
+    <col min="1" max="1" width="23.3984375" customWidth="1"/>
+    <col min="2" max="2" width="12.3984375" customWidth="1"/>
+    <col min="3" max="3" width="11.19921875" customWidth="1"/>
+    <col min="4" max="4" width="9.3984375" customWidth="1"/>
     <col min="5" max="5" width="8" customWidth="1"/>
-    <col min="6" max="7" width="9.33203125" customWidth="1"/>
+    <col min="6" max="7" width="9.3984375" customWidth="1"/>
     <col min="8" max="8" width="8" customWidth="1"/>
-    <col min="9" max="9" width="9.33203125" customWidth="1"/>
+    <col min="9" max="9" width="9.3984375" customWidth="1"/>
     <col min="10" max="10" width="14" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1" s="21" t="s">
-        <v>69</v>
-      </c>
-      <c r="B1" s="20"/>
-    </row>
-    <row r="2" spans="1:10" ht="35.450000000000003" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="A1" s="20" t="s">
+        <v>68</v>
+      </c>
+      <c r="B1" s="21"/>
+    </row>
+    <row r="2" spans="1:10" ht="35.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="16" t="s">
         <v>0</v>
       </c>
@@ -1412,7 +1367,7 @@
       <c r="I2" s="16"/>
       <c r="J2" s="16"/>
     </row>
-    <row r="3" spans="1:10" ht="18.95" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:10" ht="19" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="17" t="s">
         <v>1</v>
       </c>
@@ -1436,7 +1391,7 @@
       </c>
       <c r="H3" s="3"/>
     </row>
-    <row r="4" spans="1:10" ht="9" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:10" ht="9" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" s="18"/>
       <c r="B4" s="4" t="s">
         <v>4</v>
@@ -1458,7 +1413,7 @@
       </c>
       <c r="H4" s="6"/>
     </row>
-    <row r="5" spans="1:10" ht="8.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:10" ht="8.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A5" s="7" t="s">
         <v>5</v>
       </c>
@@ -1482,7 +1437,7 @@
       </c>
       <c r="H5" s="6"/>
     </row>
-    <row r="6" spans="1:10" ht="8.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:10" ht="8.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A6" s="7" t="s">
         <v>7</v>
       </c>
@@ -1506,7 +1461,7 @@
       </c>
       <c r="H6" s="6"/>
     </row>
-    <row r="7" spans="1:10" ht="8.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:10" ht="8.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A7" s="7" t="s">
         <v>8</v>
       </c>
@@ -1530,7 +1485,7 @@
       </c>
       <c r="H7" s="6"/>
     </row>
-    <row r="8" spans="1:10" ht="8.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:10" ht="8.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A8" s="7" t="s">
         <v>9</v>
       </c>
@@ -1554,7 +1509,7 @@
       </c>
       <c r="H8" s="6"/>
     </row>
-    <row r="9" spans="1:10" ht="8.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:10" ht="8.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A9" s="7" t="s">
         <v>10</v>
       </c>
@@ -1578,7 +1533,7 @@
       </c>
       <c r="H9" s="6"/>
     </row>
-    <row r="10" spans="1:10" ht="8.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:10" ht="8.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A10" s="7" t="s">
         <v>11</v>
       </c>
@@ -1602,7 +1557,7 @@
       </c>
       <c r="H10" s="6"/>
     </row>
-    <row r="11" spans="1:10" ht="8.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:10" ht="8.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A11" s="7" t="s">
         <v>12</v>
       </c>
@@ -1626,7 +1581,7 @@
       </c>
       <c r="H11" s="6"/>
     </row>
-    <row r="12" spans="1:10" ht="8.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:10" ht="8.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A12" s="7" t="s">
         <v>13</v>
       </c>
@@ -1650,7 +1605,7 @@
       </c>
       <c r="H12" s="6"/>
     </row>
-    <row r="13" spans="1:10" ht="8.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:10" ht="8.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A13" s="7" t="s">
         <v>14</v>
       </c>
@@ -1674,7 +1629,7 @@
       </c>
       <c r="H13" s="6"/>
     </row>
-    <row r="14" spans="1:10" ht="8.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:10" ht="8.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A14" s="7" t="s">
         <v>15</v>
       </c>
@@ -1698,7 +1653,7 @@
       </c>
       <c r="H14" s="6"/>
     </row>
-    <row r="15" spans="1:10" ht="8.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:10" ht="8.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A15" s="7" t="s">
         <v>16</v>
       </c>
@@ -1722,7 +1677,7 @@
       </c>
       <c r="H15" s="6"/>
     </row>
-    <row r="16" spans="1:10" ht="8.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:10" ht="8.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A16" s="7" t="s">
         <v>17</v>
       </c>
@@ -1746,7 +1701,7 @@
       </c>
       <c r="H16" s="6"/>
     </row>
-    <row r="17" spans="1:8" ht="8.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:8" ht="8.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A17" s="7" t="s">
         <v>18</v>
       </c>
@@ -1770,7 +1725,7 @@
       </c>
       <c r="H17" s="6"/>
     </row>
-    <row r="18" spans="1:8" ht="8.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:8" ht="8.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A18" s="7" t="s">
         <v>19</v>
       </c>
@@ -1794,7 +1749,7 @@
       </c>
       <c r="H18" s="6"/>
     </row>
-    <row r="19" spans="1:8" ht="8.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:8" ht="8.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A19" s="7" t="s">
         <v>20</v>
       </c>
@@ -1818,7 +1773,7 @@
       </c>
       <c r="H19" s="6"/>
     </row>
-    <row r="20" spans="1:8" ht="8.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:8" ht="8.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A20" s="7" t="s">
         <v>21</v>
       </c>
@@ -1842,7 +1797,7 @@
       </c>
       <c r="H20" s="6"/>
     </row>
-    <row r="21" spans="1:8" ht="8.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:8" ht="8.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A21" s="7" t="s">
         <v>22</v>
       </c>
@@ -1866,7 +1821,7 @@
       </c>
       <c r="H21" s="6"/>
     </row>
-    <row r="22" spans="1:8" ht="8.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:8" ht="8.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A22" s="7" t="s">
         <v>23</v>
       </c>
@@ -1890,7 +1845,7 @@
       </c>
       <c r="H22" s="6"/>
     </row>
-    <row r="23" spans="1:8" ht="8.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:8" ht="8.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A23" s="7" t="s">
         <v>24</v>
       </c>
@@ -1914,7 +1869,7 @@
       </c>
       <c r="H23" s="6"/>
     </row>
-    <row r="24" spans="1:8" ht="8.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:8" ht="8.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A24" s="7" t="s">
         <v>25</v>
       </c>
@@ -1938,7 +1893,7 @@
       </c>
       <c r="H24" s="6"/>
     </row>
-    <row r="25" spans="1:8" ht="8.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:8" ht="8.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A25" s="7" t="s">
         <v>26</v>
       </c>
@@ -1962,7 +1917,7 @@
       </c>
       <c r="H25" s="6"/>
     </row>
-    <row r="26" spans="1:8" ht="8.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:8" ht="8.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A26" s="7" t="s">
         <v>27</v>
       </c>
@@ -1986,7 +1941,7 @@
       </c>
       <c r="H26" s="6"/>
     </row>
-    <row r="27" spans="1:8" ht="8.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:8" ht="8.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A27" s="7" t="s">
         <v>28</v>
       </c>
@@ -2010,7 +1965,7 @@
       </c>
       <c r="H27" s="6"/>
     </row>
-    <row r="28" spans="1:8" ht="8.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:8" ht="8.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A28" s="7" t="s">
         <v>29</v>
       </c>
@@ -2034,7 +1989,7 @@
       </c>
       <c r="H28" s="6"/>
     </row>
-    <row r="29" spans="1:8" ht="8.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:8" ht="8.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A29" s="7" t="s">
         <v>30</v>
       </c>
@@ -2058,7 +2013,7 @@
       </c>
       <c r="H29" s="6"/>
     </row>
-    <row r="30" spans="1:8" ht="8.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:8" ht="8.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A30" s="7" t="s">
         <v>31</v>
       </c>
@@ -2082,7 +2037,7 @@
       </c>
       <c r="H30" s="6"/>
     </row>
-    <row r="31" spans="1:8" ht="8.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:8" ht="8.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A31" s="7" t="s">
         <v>32</v>
       </c>
@@ -2106,7 +2061,7 @@
       </c>
       <c r="H31" s="6"/>
     </row>
-    <row r="32" spans="1:8" ht="8.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:8" ht="8.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A32" s="7" t="s">
         <v>33</v>
       </c>
@@ -2130,7 +2085,7 @@
       </c>
       <c r="H32" s="6"/>
     </row>
-    <row r="33" spans="1:8" ht="8.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:8" ht="8.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A33" s="7" t="s">
         <v>34</v>
       </c>
@@ -2154,7 +2109,7 @@
       </c>
       <c r="H33" s="6"/>
     </row>
-    <row r="34" spans="1:8" ht="8.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:8" ht="8.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A34" s="7" t="s">
         <v>35</v>
       </c>
@@ -2178,7 +2133,7 @@
       </c>
       <c r="H34" s="6"/>
     </row>
-    <row r="35" spans="1:8" ht="8.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:8" ht="8.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A35" s="7" t="s">
         <v>36</v>
       </c>
@@ -2202,7 +2157,7 @@
       </c>
       <c r="H35" s="6"/>
     </row>
-    <row r="36" spans="1:8" ht="8.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:8" ht="8.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A36" s="7" t="s">
         <v>37</v>
       </c>
@@ -2226,7 +2181,7 @@
       </c>
       <c r="H36" s="6"/>
     </row>
-    <row r="37" spans="1:8" ht="8.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:8" ht="8.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A37" s="7" t="s">
         <v>38</v>
       </c>
@@ -2250,7 +2205,7 @@
       </c>
       <c r="H37" s="6"/>
     </row>
-    <row r="38" spans="1:8" ht="8.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:8" ht="8.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A38" s="7" t="s">
         <v>39</v>
       </c>
@@ -2274,7 +2229,7 @@
       </c>
       <c r="H38" s="6"/>
     </row>
-    <row r="39" spans="1:8" ht="8.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:8" ht="8.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A39" s="7" t="s">
         <v>40</v>
       </c>
@@ -2298,7 +2253,7 @@
       </c>
       <c r="H39" s="6"/>
     </row>
-    <row r="40" spans="1:8" ht="8.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:8" ht="8.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A40" s="7" t="s">
         <v>41</v>
       </c>
@@ -2322,7 +2277,7 @@
       </c>
       <c r="H40" s="6"/>
     </row>
-    <row r="41" spans="1:8" ht="8.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:8" ht="8.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A41" s="7" t="s">
         <v>42</v>
       </c>
@@ -2346,7 +2301,7 @@
       </c>
       <c r="H41" s="6"/>
     </row>
-    <row r="42" spans="1:8" ht="8.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:8" ht="8.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A42" s="7" t="s">
         <v>43</v>
       </c>
@@ -2370,7 +2325,7 @@
       </c>
       <c r="H42" s="6"/>
     </row>
-    <row r="43" spans="1:8" ht="8.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:8" ht="8.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A43" s="7" t="s">
         <v>44</v>
       </c>
@@ -2394,7 +2349,7 @@
       </c>
       <c r="H43" s="6"/>
     </row>
-    <row r="44" spans="1:8" ht="8.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:8" ht="8.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A44" s="7" t="s">
         <v>45</v>
       </c>
@@ -2418,7 +2373,7 @@
       </c>
       <c r="H44" s="6"/>
     </row>
-    <row r="45" spans="1:8" ht="8.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:8" ht="8.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A45" s="7" t="s">
         <v>46</v>
       </c>
@@ -2442,7 +2397,7 @@
       </c>
       <c r="H45" s="6"/>
     </row>
-    <row r="46" spans="1:8" ht="8.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:8" ht="8.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A46" s="7" t="s">
         <v>47</v>
       </c>
@@ -2466,7 +2421,7 @@
       </c>
       <c r="H46" s="6"/>
     </row>
-    <row r="47" spans="1:8" ht="8.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:8" ht="8.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A47" s="7" t="s">
         <v>48</v>
       </c>
@@ -2490,7 +2445,7 @@
       </c>
       <c r="H47" s="6"/>
     </row>
-    <row r="48" spans="1:8" ht="8.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:8" ht="8.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A48" s="7" t="s">
         <v>49</v>
       </c>
@@ -2514,7 +2469,7 @@
       </c>
       <c r="H48" s="6"/>
     </row>
-    <row r="49" spans="1:8" ht="8.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:8" ht="8.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A49" s="7" t="s">
         <v>50</v>
       </c>
@@ -2538,7 +2493,7 @@
       </c>
       <c r="H49" s="6"/>
     </row>
-    <row r="50" spans="1:8" ht="8.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:8" ht="8.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A50" s="7" t="s">
         <v>51</v>
       </c>
@@ -2562,7 +2517,7 @@
       </c>
       <c r="H50" s="6"/>
     </row>
-    <row r="51" spans="1:8" ht="8.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:8" ht="8.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A51" s="7" t="s">
         <v>52</v>
       </c>
@@ -2586,7 +2541,7 @@
       </c>
       <c r="H51" s="6"/>
     </row>
-    <row r="52" spans="1:8" ht="8.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:8" ht="8.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A52" s="7" t="s">
         <v>53</v>
       </c>
@@ -2610,7 +2565,7 @@
       </c>
       <c r="H52" s="6"/>
     </row>
-    <row r="53" spans="1:8" ht="8.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:8" ht="8.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A53" s="7" t="s">
         <v>54</v>
       </c>
@@ -2634,7 +2589,7 @@
       </c>
       <c r="H53" s="6"/>
     </row>
-    <row r="54" spans="1:8" ht="8.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:8" ht="8.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A54" s="7" t="s">
         <v>55</v>
       </c>
@@ -2658,7 +2613,7 @@
       </c>
       <c r="H54" s="6"/>
     </row>
-    <row r="55" spans="1:8" ht="8.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:8" ht="8.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A55" s="7" t="s">
         <v>56</v>
       </c>
@@ -2682,7 +2637,7 @@
       </c>
       <c r="H55" s="6"/>
     </row>
-    <row r="56" spans="1:8" ht="8.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:8" ht="8.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A56" s="7" t="s">
         <v>57</v>
       </c>
@@ -2706,7 +2661,7 @@
       </c>
       <c r="H56" s="6"/>
     </row>
-    <row r="57" spans="1:8" ht="8.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:8" ht="8.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A57" s="7" t="s">
         <v>58</v>
       </c>
@@ -2730,7 +2685,7 @@
       </c>
       <c r="H57" s="6"/>
     </row>
-    <row r="58" spans="1:8" ht="8.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:8" ht="8.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A58" s="7" t="s">
         <v>59</v>
       </c>
@@ -2754,7 +2709,7 @@
       </c>
       <c r="H58" s="6"/>
     </row>
-    <row r="59" spans="1:8" ht="8.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:8" ht="8.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A59" s="7" t="s">
         <v>60</v>
       </c>
@@ -2778,7 +2733,7 @@
       </c>
       <c r="H59" s="6"/>
     </row>
-    <row r="60" spans="1:8" ht="8.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:8" ht="8.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A60" s="7" t="s">
         <v>61</v>
       </c>
@@ -2802,7 +2757,7 @@
       </c>
       <c r="H60" s="6"/>
     </row>
-    <row r="61" spans="1:8" ht="8.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:8" ht="8.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A61" s="7" t="s">
         <v>62</v>
       </c>
@@ -2826,7 +2781,7 @@
       </c>
       <c r="H61" s="6"/>
     </row>
-    <row r="62" spans="1:8" ht="8.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:8" ht="8.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A62" s="7" t="s">
         <v>63</v>
       </c>
@@ -2850,7 +2805,7 @@
       </c>
       <c r="H62" s="6"/>
     </row>
-    <row r="63" spans="1:8" ht="8.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:8" ht="8.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A63" s="7" t="s">
         <v>64</v>
       </c>
@@ -2874,7 +2829,7 @@
       </c>
       <c r="H63" s="6"/>
     </row>
-    <row r="64" spans="1:8" ht="8.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:8" ht="8.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A64" s="7" t="s">
         <v>65</v>
       </c>
@@ -2898,7 +2853,7 @@
       </c>
       <c r="H64" s="6"/>
     </row>
-    <row r="65" spans="1:10" ht="8.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:10" ht="8.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A65" s="7" t="s">
         <v>66</v>
       </c>
@@ -2922,7 +2877,7 @@
       </c>
       <c r="H65" s="6"/>
     </row>
-    <row r="66" spans="1:10" ht="9.1999999999999993" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:10" ht="9.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A66" s="7" t="s">
         <v>67</v>
       </c>
@@ -2946,9 +2901,9 @@
       </c>
       <c r="H66" s="6"/>
     </row>
-    <row r="67" spans="1:10" ht="77.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A67" s="19" t="s">
-        <v>68</v>
+    <row r="67" spans="1:10" ht="77.25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A67" s="22" t="s">
+        <v>69</v>
       </c>
       <c r="B67" s="19"/>
       <c r="C67" s="19"/>

</xml_diff>